<commit_message>
komma's vervangen door punten in testdata
</commit_message>
<xml_diff>
--- a/test/data/combineer_tool/GPS_Punten.xlsx
+++ b/test/data/combineer_tool/GPS_Punten.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iris\Desktop\Bastiaan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basti\Documents\GitHub\gistools\test\data\combineer_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14715" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="23-10-2017_2_11" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="14">
   <si>
     <t>DWPCODE</t>
   </si>
@@ -58,600 +58,6 @@
     <t>PNT_soort</t>
   </si>
   <si>
-    <t>84168,4542</t>
-  </si>
-  <si>
-    <t>423012,1353</t>
-  </si>
-  <si>
-    <t>84169,6275</t>
-  </si>
-  <si>
-    <t>423011,9109</t>
-  </si>
-  <si>
-    <t>84173,496</t>
-  </si>
-  <si>
-    <t>423010,1445</t>
-  </si>
-  <si>
-    <t>84173,6214</t>
-  </si>
-  <si>
-    <t>423010,177</t>
-  </si>
-  <si>
-    <t>84188,0402</t>
-  </si>
-  <si>
-    <t>423006,6478</t>
-  </si>
-  <si>
-    <t>84187,1811</t>
-  </si>
-  <si>
-    <t>423006,5972</t>
-  </si>
-  <si>
-    <t>84181,5171</t>
-  </si>
-  <si>
-    <t>423008,0695</t>
-  </si>
-  <si>
-    <t>84181,6591</t>
-  </si>
-  <si>
-    <t>423007,8798</t>
-  </si>
-  <si>
-    <t>84132,3727</t>
-  </si>
-  <si>
-    <t>422914,6439</t>
-  </si>
-  <si>
-    <t>84131,4324</t>
-  </si>
-  <si>
-    <t>422915,3428</t>
-  </si>
-  <si>
-    <t>84131,2934</t>
-  </si>
-  <si>
-    <t>422915,4221</t>
-  </si>
-  <si>
-    <t>84120,091</t>
-  </si>
-  <si>
-    <t>422922,177</t>
-  </si>
-  <si>
-    <t>84120,9876</t>
-  </si>
-  <si>
-    <t>422921,7567</t>
-  </si>
-  <si>
-    <t>84124,2137</t>
-  </si>
-  <si>
-    <t>422919,7636</t>
-  </si>
-  <si>
-    <t>84124,501</t>
-  </si>
-  <si>
-    <t>422919,4466</t>
-  </si>
-  <si>
-    <t>84087,5129</t>
-  </si>
-  <si>
-    <t>422873,0115</t>
-  </si>
-  <si>
-    <t>84088,5215</t>
-  </si>
-  <si>
-    <t>422872,4432</t>
-  </si>
-  <si>
-    <t>84091,8671</t>
-  </si>
-  <si>
-    <t>422870,6039</t>
-  </si>
-  <si>
-    <t>84092,1205</t>
-  </si>
-  <si>
-    <t>422870,484</t>
-  </si>
-  <si>
-    <t>84112,2211</t>
-  </si>
-  <si>
-    <t>422857,5483</t>
-  </si>
-  <si>
-    <t>84111,3223</t>
-  </si>
-  <si>
-    <t>422857,8782</t>
-  </si>
-  <si>
-    <t>84109,9251</t>
-  </si>
-  <si>
-    <t>422858,4568</t>
-  </si>
-  <si>
-    <t>84109,7172</t>
-  </si>
-  <si>
-    <t>422858,5371</t>
-  </si>
-  <si>
-    <t>84013,2264</t>
-  </si>
-  <si>
-    <t>422753,6309</t>
-  </si>
-  <si>
-    <t>84014,2613</t>
-  </si>
-  <si>
-    <t>422752,8604</t>
-  </si>
-  <si>
-    <t>84016,9501</t>
-  </si>
-  <si>
-    <t>422750,3493</t>
-  </si>
-  <si>
-    <t>84017,0481</t>
-  </si>
-  <si>
-    <t>422750,346</t>
-  </si>
-  <si>
-    <t>84043,07</t>
-  </si>
-  <si>
-    <t>422731,2662</t>
-  </si>
-  <si>
-    <t>84042,3085</t>
-  </si>
-  <si>
-    <t>422732,0782</t>
-  </si>
-  <si>
-    <t>84038,3603</t>
-  </si>
-  <si>
-    <t>422735,0465</t>
-  </si>
-  <si>
-    <t>84038,2375</t>
-  </si>
-  <si>
-    <t>422735,1906</t>
-  </si>
-  <si>
-    <t>83891,5026</t>
-  </si>
-  <si>
-    <t>422602,5419</t>
-  </si>
-  <si>
-    <t>83891,018</t>
-  </si>
-  <si>
-    <t>422603,3547</t>
-  </si>
-  <si>
-    <t>83890,9339</t>
-  </si>
-  <si>
-    <t>422603,5035</t>
-  </si>
-  <si>
-    <t>83890,8442</t>
-  </si>
-  <si>
-    <t>422603,6289</t>
-  </si>
-  <si>
-    <t>83883,165</t>
-  </si>
-  <si>
-    <t>422614,6953</t>
-  </si>
-  <si>
-    <t>83883,7415</t>
-  </si>
-  <si>
-    <t>422613,8244</t>
-  </si>
-  <si>
-    <t>83885,5427</t>
-  </si>
-  <si>
-    <t>422610,8658</t>
-  </si>
-  <si>
-    <t>83885,6181</t>
-  </si>
-  <si>
-    <t>422610,7438</t>
-  </si>
-  <si>
-    <t>83817,6407</t>
-  </si>
-  <si>
-    <t>422589,5645</t>
-  </si>
-  <si>
-    <t>83817,91</t>
-  </si>
-  <si>
-    <t>422587,9473</t>
-  </si>
-  <si>
-    <t>83819,1826</t>
-  </si>
-  <si>
-    <t>422583,8756</t>
-  </si>
-  <si>
-    <t>83819,2444</t>
-  </si>
-  <si>
-    <t>422583,7389</t>
-  </si>
-  <si>
-    <t>83821,9677</t>
-  </si>
-  <si>
-    <t>422569,1701</t>
-  </si>
-  <si>
-    <t>83821,5983</t>
-  </si>
-  <si>
-    <t>422570,4978</t>
-  </si>
-  <si>
-    <t>83821,1483</t>
-  </si>
-  <si>
-    <t>422571,5605</t>
-  </si>
-  <si>
-    <t>83820,9726</t>
-  </si>
-  <si>
-    <t>422573,2623</t>
-  </si>
-  <si>
-    <t>84155,2214</t>
-  </si>
-  <si>
-    <t>422943,3141</t>
-  </si>
-  <si>
-    <t>84155,126</t>
-  </si>
-  <si>
-    <t>422943,3194</t>
-  </si>
-  <si>
-    <t>84155,6307</t>
-  </si>
-  <si>
-    <t>422943,1025</t>
-  </si>
-  <si>
-    <t>84156,7525</t>
-  </si>
-  <si>
-    <t>422942,6269</t>
-  </si>
-  <si>
-    <t>84169,8473</t>
-  </si>
-  <si>
-    <t>422936,0329</t>
-  </si>
-  <si>
-    <t>84168,995</t>
-  </si>
-  <si>
-    <t>422936,5643</t>
-  </si>
-  <si>
-    <t>84166,1157</t>
-  </si>
-  <si>
-    <t>422937,8415</t>
-  </si>
-  <si>
-    <t>84165,9436</t>
-  </si>
-  <si>
-    <t>422938,1157</t>
-  </si>
-  <si>
-    <t>84007,4726</t>
-  </si>
-  <si>
-    <t>422714,9134</t>
-  </si>
-  <si>
-    <t>84008,0334</t>
-  </si>
-  <si>
-    <t>422714,4319</t>
-  </si>
-  <si>
-    <t>84008,0856</t>
-  </si>
-  <si>
-    <t>422714,3204</t>
-  </si>
-  <si>
-    <t>84008,2092</t>
-  </si>
-  <si>
-    <t>422714,1753</t>
-  </si>
-  <si>
-    <t>84019,5896</t>
-  </si>
-  <si>
-    <t>422703,7864</t>
-  </si>
-  <si>
-    <t>84018,7382</t>
-  </si>
-  <si>
-    <t>422704,3819</t>
-  </si>
-  <si>
-    <t>84016,6236</t>
-  </si>
-  <si>
-    <t>422706,2776</t>
-  </si>
-  <si>
-    <t>84016,5395</t>
-  </si>
-  <si>
-    <t>422706,7398</t>
-  </si>
-  <si>
-    <t>83975,6497</t>
-  </si>
-  <si>
-    <t>422673,6896</t>
-  </si>
-  <si>
-    <t>83985,1644</t>
-  </si>
-  <si>
-    <t>422664,3607</t>
-  </si>
-  <si>
-    <t>83984,5149</t>
-  </si>
-  <si>
-    <t>422664,6948</t>
-  </si>
-  <si>
-    <t>83981,9948</t>
-  </si>
-  <si>
-    <t>422667,1834</t>
-  </si>
-  <si>
-    <t>83982,0123</t>
-  </si>
-  <si>
-    <t>422667,4903</t>
-  </si>
-  <si>
-    <t>83915,9568</t>
-  </si>
-  <si>
-    <t>422591,9883</t>
-  </si>
-  <si>
-    <t>83915,2133</t>
-  </si>
-  <si>
-    <t>422592,742</t>
-  </si>
-  <si>
-    <t>83911,9558</t>
-  </si>
-  <si>
-    <t>422595,536</t>
-  </si>
-  <si>
-    <t>83945,9247</t>
-  </si>
-  <si>
-    <t>422644,882</t>
-  </si>
-  <si>
-    <t>83945,2099</t>
-  </si>
-  <si>
-    <t>422643,9438</t>
-  </si>
-  <si>
-    <t>83945,1838</t>
-  </si>
-  <si>
-    <t>422643,802</t>
-  </si>
-  <si>
-    <t>83945,1317</t>
-  </si>
-  <si>
-    <t>422643,6213</t>
-  </si>
-  <si>
-    <t>83877,9576</t>
-  </si>
-  <si>
-    <t>422578,7508</t>
-  </si>
-  <si>
-    <t>83876,99</t>
-  </si>
-  <si>
-    <t>422578,9863</t>
-  </si>
-  <si>
-    <t>83876,7157</t>
-  </si>
-  <si>
-    <t>422579,034</t>
-  </si>
-  <si>
-    <t>83876,5099</t>
-  </si>
-  <si>
-    <t>422578,9107</t>
-  </si>
-  <si>
-    <t>83864,142</t>
-  </si>
-  <si>
-    <t>422580,1894</t>
-  </si>
-  <si>
-    <t>83865,4725</t>
-  </si>
-  <si>
-    <t>422580,1593</t>
-  </si>
-  <si>
-    <t>83867,1802</t>
-  </si>
-  <si>
-    <t>422579,9352</t>
-  </si>
-  <si>
-    <t>83867,7121</t>
-  </si>
-  <si>
-    <t>422579,9541</t>
-  </si>
-  <si>
-    <t>88369,5651</t>
-  </si>
-  <si>
-    <t>429298,904</t>
-  </si>
-  <si>
-    <t>88370,327</t>
-  </si>
-  <si>
-    <t>429298,6809</t>
-  </si>
-  <si>
-    <t>88371,5478</t>
-  </si>
-  <si>
-    <t>429298,2515</t>
-  </si>
-  <si>
-    <t>88371,6554</t>
-  </si>
-  <si>
-    <t>429298,1821</t>
-  </si>
-  <si>
-    <t>88377,6642</t>
-  </si>
-  <si>
-    <t>429294,4657</t>
-  </si>
-  <si>
-    <t>88376,6815</t>
-  </si>
-  <si>
-    <t>429294,7494</t>
-  </si>
-  <si>
-    <t>88375,7054</t>
-  </si>
-  <si>
-    <t>429295,8212</t>
-  </si>
-  <si>
-    <t>88375,7855</t>
-  </si>
-  <si>
-    <t>429295,7266</t>
-  </si>
-  <si>
-    <t>88373,7347</t>
-  </si>
-  <si>
-    <t>429317,208</t>
-  </si>
-  <si>
-    <t>88375,0041</t>
-  </si>
-  <si>
-    <t>429317,252</t>
-  </si>
-  <si>
-    <t>88376,4093</t>
-  </si>
-  <si>
-    <t>429317,2529</t>
-  </si>
-  <si>
-    <t>88376,5302</t>
-  </si>
-  <si>
-    <t>429317,2528</t>
-  </si>
-  <si>
-    <t>88387,7888</t>
-  </si>
-  <si>
-    <t>429318,1723</t>
-  </si>
-  <si>
-    <t>88387,1408</t>
-  </si>
-  <si>
-    <t>429318,096</t>
-  </si>
-  <si>
-    <t>88385,5607</t>
-  </si>
-  <si>
-    <t>429318,1685</t>
-  </si>
-  <si>
-    <t>88385,2309</t>
-  </si>
-  <si>
-    <t>429318,1732</t>
-  </si>
-  <si>
     <t>Maaiveld</t>
   </si>
   <si>
@@ -664,7 +70,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -1505,11 +911,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1556,17 +962,17 @@
       <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
+      <c r="D2" s="2">
+        <v>84168.454199999993</v>
+      </c>
+      <c r="E2" s="2">
+        <v>423012.13530000002</v>
       </c>
       <c r="F2" s="2">
         <v>-0.43630000000000002</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1579,17 +985,17 @@
       <c r="C3" s="1">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
+      <c r="D3" s="2">
+        <v>84169.627500000002</v>
+      </c>
+      <c r="E3" s="2">
+        <v>423011.91090000002</v>
       </c>
       <c r="F3" s="2">
         <v>-0.433</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1602,17 +1008,17 @@
       <c r="C4" s="1">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>16</v>
+      <c r="D4" s="2">
+        <v>84173.495999999999</v>
+      </c>
+      <c r="E4" s="2">
+        <v>423010.14449999999</v>
       </c>
       <c r="F4" s="2">
         <v>-1.6478999999999999</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1625,11 +1031,11 @@
       <c r="C5" s="1">
         <v>4</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>18</v>
+      <c r="D5" s="2">
+        <v>84173.621400000004</v>
+      </c>
+      <c r="E5" s="2">
+        <v>423010.17700000003</v>
       </c>
       <c r="F5" s="2">
         <v>-1.7998000000000001</v>
@@ -1648,17 +1054,17 @@
       <c r="C6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>20</v>
+      <c r="D6" s="2">
+        <v>84188.040200000003</v>
+      </c>
+      <c r="E6" s="2">
+        <v>423006.64779999998</v>
       </c>
       <c r="F6" s="2">
         <v>-0.43469999999999998</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1671,17 +1077,17 @@
       <c r="C7" s="1">
         <v>2</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>22</v>
+      <c r="D7" s="2">
+        <v>84187.181100000002</v>
+      </c>
+      <c r="E7" s="2">
+        <v>423006.59720000002</v>
       </c>
       <c r="F7" s="2">
         <v>-0.73770000000000002</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1694,17 +1100,17 @@
       <c r="C8" s="1">
         <v>3</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>24</v>
+      <c r="D8" s="2">
+        <v>84181.517099999997</v>
+      </c>
+      <c r="E8" s="2">
+        <v>423008.06949999998</v>
       </c>
       <c r="F8" s="2">
         <v>-1.7544</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1717,11 +1123,11 @@
       <c r="C9" s="1">
         <v>4</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>26</v>
+      <c r="D9" s="2">
+        <v>84181.659100000004</v>
+      </c>
+      <c r="E9" s="2">
+        <v>423007.8798</v>
       </c>
       <c r="F9" s="2">
         <v>-1.8237000000000001</v>
@@ -1740,17 +1146,17 @@
       <c r="C10" s="1">
         <v>2</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>28</v>
+      <c r="D10" s="2">
+        <v>84132.372700000007</v>
+      </c>
+      <c r="E10" s="2">
+        <v>422914.64390000002</v>
       </c>
       <c r="F10" s="2">
         <v>-1.6269</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1763,17 +1169,17 @@
       <c r="C11" s="1">
         <v>3</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>30</v>
+      <c r="D11" s="2">
+        <v>84131.432400000005</v>
+      </c>
+      <c r="E11" s="2">
+        <v>422915.34279999998</v>
       </c>
       <c r="F11" s="2">
         <v>-1.6617</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1786,11 +1192,11 @@
       <c r="C12" s="1">
         <v>4</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>32</v>
+      <c r="D12" s="2">
+        <v>84131.293399999995</v>
+      </c>
+      <c r="E12" s="2">
+        <v>422915.42210000003</v>
       </c>
       <c r="F12" s="2">
         <v>-1.7966</v>
@@ -1809,17 +1215,17 @@
       <c r="C13" s="1">
         <v>1</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>34</v>
+      <c r="D13" s="2">
+        <v>84120.091</v>
+      </c>
+      <c r="E13" s="2">
+        <v>422922.17700000003</v>
       </c>
       <c r="F13" s="2">
         <v>-0.35659999999999997</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1832,17 +1238,17 @@
       <c r="C14" s="1">
         <v>2</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>36</v>
+      <c r="D14" s="2">
+        <v>84120.987599999993</v>
+      </c>
+      <c r="E14" s="2">
+        <v>422921.75670000003</v>
       </c>
       <c r="F14" s="2">
         <v>-0.26340000000000002</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1855,17 +1261,17 @@
       <c r="C15" s="1">
         <v>3</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>38</v>
+      <c r="D15" s="2">
+        <v>84124.213699999993</v>
+      </c>
+      <c r="E15" s="2">
+        <v>422919.76360000001</v>
       </c>
       <c r="F15" s="2">
         <v>-1.6619999999999999</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1878,11 +1284,11 @@
       <c r="C16" s="1">
         <v>4</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>40</v>
+      <c r="D16" s="2">
+        <v>84124.501000000004</v>
+      </c>
+      <c r="E16" s="2">
+        <v>422919.44660000002</v>
       </c>
       <c r="F16" s="2">
         <v>-1.7968999999999999</v>
@@ -1901,17 +1307,17 @@
       <c r="C17" s="1">
         <v>1</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>42</v>
+      <c r="D17" s="2">
+        <v>84087.512900000002</v>
+      </c>
+      <c r="E17" s="2">
+        <v>422873.01150000002</v>
       </c>
       <c r="F17" s="2">
         <v>-0.44</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1924,17 +1330,17 @@
       <c r="C18" s="1">
         <v>2</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>44</v>
+      <c r="D18" s="2">
+        <v>84088.521500000003</v>
+      </c>
+      <c r="E18" s="2">
+        <v>422872.44319999998</v>
       </c>
       <c r="F18" s="2">
         <v>-0.3508</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1947,17 +1353,17 @@
       <c r="C19" s="1">
         <v>3</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>46</v>
+      <c r="D19" s="2">
+        <v>84091.867100000003</v>
+      </c>
+      <c r="E19" s="2">
+        <v>422870.60389999999</v>
       </c>
       <c r="F19" s="2">
         <v>-1.7275</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1970,11 +1376,11 @@
       <c r="C20" s="1">
         <v>4</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>48</v>
+      <c r="D20" s="2">
+        <v>84092.120500000005</v>
+      </c>
+      <c r="E20" s="2">
+        <v>422870.484</v>
       </c>
       <c r="F20" s="2">
         <v>-1.8023</v>
@@ -1993,17 +1399,17 @@
       <c r="C21" s="1">
         <v>1</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>50</v>
+      <c r="D21" s="2">
+        <v>84112.221099999995</v>
+      </c>
+      <c r="E21" s="2">
+        <v>422857.54830000002</v>
       </c>
       <c r="F21" s="2">
         <v>-1.5039</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2016,17 +1422,17 @@
       <c r="C22" s="1">
         <v>2</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>52</v>
+      <c r="D22" s="2">
+        <v>84111.3223</v>
+      </c>
+      <c r="E22" s="2">
+        <v>422857.87819999998</v>
       </c>
       <c r="F22" s="2">
         <v>-1.5958000000000001</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -2039,17 +1445,17 @@
       <c r="C23" s="1">
         <v>3</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>54</v>
+      <c r="D23" s="2">
+        <v>84109.925099999993</v>
+      </c>
+      <c r="E23" s="2">
+        <v>422858.45679999999</v>
       </c>
       <c r="F23" s="2">
         <v>-1.7789999999999999</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2062,11 +1468,11 @@
       <c r="C24" s="1">
         <v>4</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>56</v>
+      <c r="D24" s="2">
+        <v>84109.717199999999</v>
+      </c>
+      <c r="E24" s="2">
+        <v>422858.53710000002</v>
       </c>
       <c r="F24" s="2">
         <v>-1.7779</v>
@@ -2085,17 +1491,17 @@
       <c r="C25" s="1">
         <v>1</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>58</v>
+      <c r="D25" s="2">
+        <v>84013.2264</v>
+      </c>
+      <c r="E25" s="2">
+        <v>422753.63089999999</v>
       </c>
       <c r="F25" s="2">
         <v>-0.67920000000000003</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2108,17 +1514,17 @@
       <c r="C26" s="1">
         <v>2</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>60</v>
+      <c r="D26" s="2">
+        <v>84014.261299999998</v>
+      </c>
+      <c r="E26" s="2">
+        <v>422752.86040000001</v>
       </c>
       <c r="F26" s="2">
         <v>-0.69</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -2131,17 +1537,17 @@
       <c r="C27" s="1">
         <v>3</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>62</v>
+      <c r="D27" s="2">
+        <v>84016.950100000002</v>
+      </c>
+      <c r="E27" s="2">
+        <v>422750.3493</v>
       </c>
       <c r="F27" s="2">
         <v>-1.6492</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2154,11 +1560,11 @@
       <c r="C28" s="1">
         <v>4</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>64</v>
+      <c r="D28" s="2">
+        <v>84017.0481</v>
+      </c>
+      <c r="E28" s="2">
+        <v>422750.34600000002</v>
       </c>
       <c r="F28" s="2">
         <v>-1.7837000000000001</v>
@@ -2177,17 +1583,17 @@
       <c r="C29" s="1">
         <v>1</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>66</v>
+      <c r="D29" s="2">
+        <v>84043.07</v>
+      </c>
+      <c r="E29" s="2">
+        <v>422731.26620000001</v>
       </c>
       <c r="F29" s="2">
         <v>-0.81420000000000003</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2200,17 +1606,17 @@
       <c r="C30" s="1">
         <v>2</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>68</v>
+      <c r="D30" s="2">
+        <v>84042.308499999999</v>
+      </c>
+      <c r="E30" s="2">
+        <v>422732.07819999999</v>
       </c>
       <c r="F30" s="2">
         <v>-0.79369999999999996</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2223,17 +1629,17 @@
       <c r="C31" s="1">
         <v>3</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>70</v>
+      <c r="D31" s="2">
+        <v>84038.3603</v>
+      </c>
+      <c r="E31" s="2">
+        <v>422735.0465</v>
       </c>
       <c r="F31" s="2">
         <v>-1.8058000000000001</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2246,11 +1652,11 @@
       <c r="C32" s="1">
         <v>4</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>72</v>
+      <c r="D32" s="2">
+        <v>84038.237500000003</v>
+      </c>
+      <c r="E32" s="2">
+        <v>422735.19059999997</v>
       </c>
       <c r="F32" s="2">
         <v>-1.8279000000000001</v>
@@ -2269,17 +1675,17 @@
       <c r="C33" s="1">
         <v>1</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>74</v>
+      <c r="D33" s="2">
+        <v>83891.502600000007</v>
+      </c>
+      <c r="E33" s="2">
+        <v>422602.54190000001</v>
       </c>
       <c r="F33" s="2">
         <v>-1.8865000000000001</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2292,17 +1698,17 @@
       <c r="C34" s="1">
         <v>2</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>76</v>
+      <c r="D34" s="2">
+        <v>83891.017999999996</v>
+      </c>
+      <c r="E34" s="2">
+        <v>422603.35470000003</v>
       </c>
       <c r="F34" s="2">
         <v>-1.7589999999999999</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -2315,17 +1721,17 @@
       <c r="C35" s="1">
         <v>3</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>78</v>
+      <c r="D35" s="2">
+        <v>83890.933900000004</v>
+      </c>
+      <c r="E35" s="2">
+        <v>422603.50349999999</v>
       </c>
       <c r="F35" s="2">
         <v>-1.7216</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -2338,11 +1744,11 @@
       <c r="C36" s="1">
         <v>4</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>80</v>
+      <c r="D36" s="2">
+        <v>83890.844200000007</v>
+      </c>
+      <c r="E36" s="2">
+        <v>422603.62890000001</v>
       </c>
       <c r="F36" s="2">
         <v>-1.8022</v>
@@ -2361,17 +1767,17 @@
       <c r="C37" s="1">
         <v>1</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>82</v>
+      <c r="D37" s="2">
+        <v>83883.164999999994</v>
+      </c>
+      <c r="E37" s="2">
+        <v>422614.69530000002</v>
       </c>
       <c r="F37" s="2">
         <v>-0.71909999999999996</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2384,17 +1790,17 @@
       <c r="C38" s="1">
         <v>2</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>84</v>
+      <c r="D38" s="2">
+        <v>83883.741500000004</v>
+      </c>
+      <c r="E38" s="2">
+        <v>422613.82439999998</v>
       </c>
       <c r="F38" s="2">
         <v>-0.79549999999999998</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2407,17 +1813,17 @@
       <c r="C39" s="1">
         <v>3</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>86</v>
+      <c r="D39" s="2">
+        <v>83885.542700000005</v>
+      </c>
+      <c r="E39" s="2">
+        <v>422610.86580000003</v>
       </c>
       <c r="F39" s="2">
         <v>-1.7076</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2430,11 +1836,11 @@
       <c r="C40" s="1">
         <v>4</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>88</v>
+      <c r="D40" s="2">
+        <v>83885.618100000007</v>
+      </c>
+      <c r="E40" s="2">
+        <v>422610.7438</v>
       </c>
       <c r="F40" s="2">
         <v>-1.7990999999999999</v>
@@ -2453,17 +1859,17 @@
       <c r="C41" s="1">
         <v>1</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>90</v>
+      <c r="D41" s="2">
+        <v>83817.640700000004</v>
+      </c>
+      <c r="E41" s="2">
+        <v>422589.56449999998</v>
       </c>
       <c r="F41" s="2">
         <v>-0.17580000000000001</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2476,17 +1882,17 @@
       <c r="C42" s="1">
         <v>2</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>92</v>
+      <c r="D42" s="2">
+        <v>83817.91</v>
+      </c>
+      <c r="E42" s="2">
+        <v>422587.9473</v>
       </c>
       <c r="F42" s="2">
         <v>-0.19789999999999999</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2499,17 +1905,17 @@
       <c r="C43" s="1">
         <v>3</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>94</v>
+      <c r="D43" s="2">
+        <v>83819.1826</v>
+      </c>
+      <c r="E43" s="2">
+        <v>422583.87560000003</v>
       </c>
       <c r="F43" s="2">
         <v>-1.7323</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2522,11 +1928,11 @@
       <c r="C44" s="1">
         <v>4</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>96</v>
+      <c r="D44" s="2">
+        <v>83819.244399999996</v>
+      </c>
+      <c r="E44" s="2">
+        <v>422583.7389</v>
       </c>
       <c r="F44" s="2">
         <v>-1.7621</v>
@@ -2545,17 +1951,17 @@
       <c r="C45" s="1">
         <v>1</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>98</v>
+      <c r="D45" s="2">
+        <v>83821.967699999994</v>
+      </c>
+      <c r="E45" s="2">
+        <v>422569.17009999999</v>
       </c>
       <c r="F45" s="2">
         <v>-0.85960000000000003</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -2568,17 +1974,17 @@
       <c r="C46" s="1">
         <v>2</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>100</v>
+      <c r="D46" s="2">
+        <v>83821.598299999998</v>
+      </c>
+      <c r="E46" s="2">
+        <v>422570.49780000001</v>
       </c>
       <c r="F46" s="2">
         <v>-0.87890000000000001</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2591,17 +1997,17 @@
       <c r="C47" s="1">
         <v>3</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>102</v>
+      <c r="D47" s="2">
+        <v>83821.148300000001</v>
+      </c>
+      <c r="E47" s="2">
+        <v>422571.56050000002</v>
       </c>
       <c r="F47" s="2">
         <v>-1.712</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2614,11 +2020,11 @@
       <c r="C48" s="1">
         <v>4</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>104</v>
+      <c r="D48" s="2">
+        <v>83820.972599999994</v>
+      </c>
+      <c r="E48" s="2">
+        <v>422573.2623</v>
       </c>
       <c r="F48" s="2">
         <v>-1.7855000000000001</v>
@@ -2637,17 +2043,17 @@
       <c r="C49" s="1">
         <v>1</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>106</v>
+      <c r="D49" s="2">
+        <v>84155.221399999995</v>
+      </c>
+      <c r="E49" s="2">
+        <v>422943.31410000002</v>
       </c>
       <c r="F49" s="2">
         <v>-1.5725</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2660,17 +2066,17 @@
       <c r="C50" s="1">
         <v>2</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>108</v>
+      <c r="D50" s="2">
+        <v>84155.126000000004</v>
+      </c>
+      <c r="E50" s="2">
+        <v>422943.31939999998</v>
       </c>
       <c r="F50" s="2">
         <v>-1.5995999999999999</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2683,17 +2089,17 @@
       <c r="C51" s="1">
         <v>3</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>110</v>
+      <c r="D51" s="2">
+        <v>84155.630699999994</v>
+      </c>
+      <c r="E51" s="2">
+        <v>422943.10249999998</v>
       </c>
       <c r="F51" s="2">
         <v>-1.8169</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2706,11 +2112,11 @@
       <c r="C52" s="1">
         <v>4</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>112</v>
+      <c r="D52" s="2">
+        <v>84156.752500000002</v>
+      </c>
+      <c r="E52" s="2">
+        <v>422942.62689999997</v>
       </c>
       <c r="F52" s="2">
         <v>-1.7912999999999999</v>
@@ -2729,17 +2135,17 @@
       <c r="C53" s="1">
         <v>1</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>114</v>
+      <c r="D53" s="2">
+        <v>84169.847299999994</v>
+      </c>
+      <c r="E53" s="2">
+        <v>422936.03289999999</v>
       </c>
       <c r="F53" s="2">
         <v>-0.71140000000000003</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2752,17 +2158,17 @@
       <c r="C54" s="1">
         <v>2</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>116</v>
+      <c r="D54" s="2">
+        <v>84168.994999999995</v>
+      </c>
+      <c r="E54" s="2">
+        <v>422936.56430000003</v>
       </c>
       <c r="F54" s="2">
         <v>-0.68669999999999998</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2775,17 +2181,17 @@
       <c r="C55" s="1">
         <v>3</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>118</v>
+      <c r="D55" s="2">
+        <v>84166.115699999995</v>
+      </c>
+      <c r="E55" s="2">
+        <v>422937.84149999998</v>
       </c>
       <c r="F55" s="2">
         <v>-1.7677</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2798,11 +2204,11 @@
       <c r="C56" s="1">
         <v>4</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>120</v>
+      <c r="D56" s="2">
+        <v>84165.943599999999</v>
+      </c>
+      <c r="E56" s="2">
+        <v>422938.11570000002</v>
       </c>
       <c r="F56" s="2">
         <v>-1.794</v>
@@ -2821,17 +2227,17 @@
       <c r="C57" s="1">
         <v>1</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>122</v>
+      <c r="D57" s="2">
+        <v>84007.472599999994</v>
+      </c>
+      <c r="E57" s="2">
+        <v>422714.91340000002</v>
       </c>
       <c r="F57" s="2">
         <v>-1.7205999999999999</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2844,17 +2250,17 @@
       <c r="C58" s="1">
         <v>2</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>124</v>
+      <c r="D58" s="2">
+        <v>84008.0334</v>
+      </c>
+      <c r="E58" s="2">
+        <v>422714.43190000003</v>
       </c>
       <c r="F58" s="2">
         <v>-1.7507999999999999</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2867,17 +2273,17 @@
       <c r="C59" s="1">
         <v>3</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>126</v>
+      <c r="D59" s="2">
+        <v>84008.085600000006</v>
+      </c>
+      <c r="E59" s="2">
+        <v>422714.32040000003</v>
       </c>
       <c r="F59" s="2">
         <v>-1.6369</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2890,11 +2296,11 @@
       <c r="C60" s="1">
         <v>4</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>128</v>
+      <c r="D60" s="2">
+        <v>84008.209199999998</v>
+      </c>
+      <c r="E60" s="2">
+        <v>422714.1753</v>
       </c>
       <c r="F60" s="2">
         <v>-1.8309</v>
@@ -2913,17 +2319,17 @@
       <c r="C61" s="1">
         <v>1</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>130</v>
+      <c r="D61" s="2">
+        <v>84019.589600000007</v>
+      </c>
+      <c r="E61" s="2">
+        <v>422703.78639999998</v>
       </c>
       <c r="F61" s="2">
         <v>-0.79649999999999999</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2936,17 +2342,17 @@
       <c r="C62" s="1">
         <v>2</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>132</v>
+      <c r="D62" s="2">
+        <v>84018.738200000007</v>
+      </c>
+      <c r="E62" s="2">
+        <v>422704.38189999998</v>
       </c>
       <c r="F62" s="2">
         <v>-0.72699999999999998</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2959,17 +2365,17 @@
       <c r="C63" s="1">
         <v>3</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>134</v>
+      <c r="D63" s="2">
+        <v>84016.623600000006</v>
+      </c>
+      <c r="E63" s="2">
+        <v>422706.27759999997</v>
       </c>
       <c r="F63" s="2">
         <v>-1.8041</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2982,11 +2388,11 @@
       <c r="C64" s="1">
         <v>4</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>136</v>
+      <c r="D64" s="2">
+        <v>84016.539499999999</v>
+      </c>
+      <c r="E64" s="2">
+        <v>422706.73979999998</v>
       </c>
       <c r="F64" s="2">
         <v>-1.7297</v>
@@ -3005,11 +2411,11 @@
       <c r="C65" s="1">
         <v>4</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>138</v>
+      <c r="D65" s="2">
+        <v>83975.649699999994</v>
+      </c>
+      <c r="E65" s="2">
+        <v>422673.68959999998</v>
       </c>
       <c r="F65" s="2">
         <v>-1.8955</v>
@@ -3028,17 +2434,17 @@
       <c r="C66" s="1">
         <v>1</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>140</v>
+      <c r="D66" s="2">
+        <v>83985.164399999994</v>
+      </c>
+      <c r="E66" s="2">
+        <v>422664.36070000002</v>
       </c>
       <c r="F66" s="2">
         <v>-0.85319999999999996</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -3051,17 +2457,17 @@
       <c r="C67" s="1">
         <v>2</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>142</v>
+      <c r="D67" s="2">
+        <v>83984.514899999995</v>
+      </c>
+      <c r="E67" s="2">
+        <v>422664.6948</v>
       </c>
       <c r="F67" s="2">
         <v>-0.8458</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -3074,17 +2480,17 @@
       <c r="C68" s="1">
         <v>3</v>
       </c>
-      <c r="D68" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>144</v>
+      <c r="D68" s="2">
+        <v>83981.9948</v>
+      </c>
+      <c r="E68" s="2">
+        <v>422667.18339999998</v>
       </c>
       <c r="F68" s="2">
         <v>-1.7669999999999999</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -3097,11 +2503,11 @@
       <c r="C69" s="1">
         <v>4</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>146</v>
+      <c r="D69" s="2">
+        <v>83982.012300000002</v>
+      </c>
+      <c r="E69" s="2">
+        <v>422667.4903</v>
       </c>
       <c r="F69" s="2">
         <v>-1.8544</v>
@@ -3120,17 +2526,17 @@
       <c r="C70" s="1">
         <v>1</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>148</v>
+      <c r="D70" s="2">
+        <v>83915.9568</v>
+      </c>
+      <c r="E70" s="2">
+        <v>422591.98830000003</v>
       </c>
       <c r="F70" s="2">
         <v>-0.72099999999999997</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -3143,17 +2549,17 @@
       <c r="C71" s="1">
         <v>2</v>
       </c>
-      <c r="D71" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>150</v>
+      <c r="D71" s="2">
+        <v>83915.213300000003</v>
+      </c>
+      <c r="E71" s="2">
+        <v>422592.74200000003</v>
       </c>
       <c r="F71" s="2">
         <v>-0.82110000000000005</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -3166,17 +2572,17 @@
       <c r="C72" s="1">
         <v>3</v>
       </c>
-      <c r="D72" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>152</v>
+      <c r="D72" s="2">
+        <v>83911.955799999996</v>
+      </c>
+      <c r="E72" s="2">
+        <v>422595.53600000002</v>
       </c>
       <c r="F72" s="2">
         <v>-1.8259000000000001</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -3189,17 +2595,17 @@
       <c r="C73" s="1">
         <v>1</v>
       </c>
-      <c r="D73" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>154</v>
+      <c r="D73" s="2">
+        <v>83945.924700000003</v>
+      </c>
+      <c r="E73" s="2">
+        <v>422644.88199999998</v>
       </c>
       <c r="F73" s="2">
         <v>-1.7143999999999999</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -3212,17 +2618,17 @@
       <c r="C74" s="1">
         <v>2</v>
       </c>
-      <c r="D74" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>156</v>
+      <c r="D74" s="2">
+        <v>83945.209900000002</v>
+      </c>
+      <c r="E74" s="2">
+        <v>422643.94380000001</v>
       </c>
       <c r="F74" s="2">
         <v>-1.6899</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -3235,17 +2641,17 @@
       <c r="C75" s="1">
         <v>3</v>
       </c>
-      <c r="D75" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>158</v>
+      <c r="D75" s="2">
+        <v>83945.183799999999</v>
+      </c>
+      <c r="E75" s="2">
+        <v>422643.80200000003</v>
       </c>
       <c r="F75" s="2">
         <v>-1.7079</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -3258,11 +2664,11 @@
       <c r="C76" s="1">
         <v>4</v>
       </c>
-      <c r="D76" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>160</v>
+      <c r="D76" s="2">
+        <v>83945.131699999998</v>
+      </c>
+      <c r="E76" s="2">
+        <v>422643.6213</v>
       </c>
       <c r="F76" s="2">
         <v>-1.8192999999999999</v>
@@ -3281,17 +2687,17 @@
       <c r="C77" s="1">
         <v>1</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>162</v>
+      <c r="D77" s="2">
+        <v>83877.957599999994</v>
+      </c>
+      <c r="E77" s="2">
+        <v>422578.75079999998</v>
       </c>
       <c r="F77" s="2">
         <v>-1.7352000000000001</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -3304,17 +2710,17 @@
       <c r="C78" s="1">
         <v>2</v>
       </c>
-      <c r="D78" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>164</v>
+      <c r="D78" s="2">
+        <v>83876.990000000005</v>
+      </c>
+      <c r="E78" s="2">
+        <v>422578.98629999999</v>
       </c>
       <c r="F78" s="2">
         <v>-1.722</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -3327,17 +2733,17 @@
       <c r="C79" s="1">
         <v>3</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>166</v>
+      <c r="D79" s="2">
+        <v>83876.715700000001</v>
+      </c>
+      <c r="E79" s="2">
+        <v>422579.03399999999</v>
       </c>
       <c r="F79" s="2">
         <v>-1.6146</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -3350,11 +2756,11 @@
       <c r="C80" s="1">
         <v>4</v>
       </c>
-      <c r="D80" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>168</v>
+      <c r="D80" s="2">
+        <v>83876.509900000005</v>
+      </c>
+      <c r="E80" s="2">
+        <v>422578.91070000001</v>
       </c>
       <c r="F80" s="2">
         <v>-1.8065</v>
@@ -3373,17 +2779,17 @@
       <c r="C81" s="1">
         <v>1</v>
       </c>
-      <c r="D81" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>170</v>
+      <c r="D81" s="2">
+        <v>83864.142000000007</v>
+      </c>
+      <c r="E81" s="2">
+        <v>422580.18939999997</v>
       </c>
       <c r="F81" s="2">
         <v>-1.0617000000000001</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -3396,17 +2802,17 @@
       <c r="C82" s="1">
         <v>2</v>
       </c>
-      <c r="D82" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>172</v>
+      <c r="D82" s="2">
+        <v>83865.472500000003</v>
+      </c>
+      <c r="E82" s="2">
+        <v>422580.1593</v>
       </c>
       <c r="F82" s="2">
         <v>-1.0726</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -3419,17 +2825,17 @@
       <c r="C83" s="1">
         <v>3</v>
       </c>
-      <c r="D83" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>174</v>
+      <c r="D83" s="2">
+        <v>83867.180200000003</v>
+      </c>
+      <c r="E83" s="2">
+        <v>422579.93520000001</v>
       </c>
       <c r="F83" s="2">
         <v>-1.6423000000000001</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -3442,11 +2848,11 @@
       <c r="C84" s="1">
         <v>4</v>
       </c>
-      <c r="D84" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>176</v>
+      <c r="D84" s="2">
+        <v>83867.712100000004</v>
+      </c>
+      <c r="E84" s="2">
+        <v>422579.95409999997</v>
       </c>
       <c r="F84" s="2">
         <v>-1.79</v>
@@ -3465,17 +2871,17 @@
       <c r="C85" s="1">
         <v>1</v>
       </c>
-      <c r="D85" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>178</v>
+      <c r="D85" s="2">
+        <v>88369.565100000007</v>
+      </c>
+      <c r="E85" s="2">
+        <v>429298.90399999998</v>
       </c>
       <c r="F85" s="2">
         <v>0.48749999999999999</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -3488,17 +2894,17 @@
       <c r="C86" s="1">
         <v>2</v>
       </c>
-      <c r="D86" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>180</v>
+      <c r="D86" s="2">
+        <v>88370.327000000005</v>
+      </c>
+      <c r="E86" s="2">
+        <v>429298.68089999998</v>
       </c>
       <c r="F86" s="2">
         <v>0.41449999999999998</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -3511,17 +2917,17 @@
       <c r="C87" s="1">
         <v>3</v>
       </c>
-      <c r="D87" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>182</v>
+      <c r="D87" s="2">
+        <v>88371.5478</v>
+      </c>
+      <c r="E87" s="2">
+        <v>429298.25150000001</v>
       </c>
       <c r="F87" s="2">
         <v>-0.17480000000000001</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -3534,11 +2940,11 @@
       <c r="C88" s="1">
         <v>4</v>
       </c>
-      <c r="D88" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>184</v>
+      <c r="D88" s="2">
+        <v>88371.655400000003</v>
+      </c>
+      <c r="E88" s="2">
+        <v>429298.18209999998</v>
       </c>
       <c r="F88" s="2">
         <v>-0.3715</v>
@@ -3557,17 +2963,17 @@
       <c r="C89" s="1">
         <v>1</v>
       </c>
-      <c r="D89" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>186</v>
+      <c r="D89" s="2">
+        <v>88377.664199999999</v>
+      </c>
+      <c r="E89" s="2">
+        <v>429294.4657</v>
       </c>
       <c r="F89" s="2">
         <v>0.42480000000000001</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -3580,17 +2986,17 @@
       <c r="C90" s="1">
         <v>2</v>
       </c>
-      <c r="D90" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>188</v>
+      <c r="D90" s="2">
+        <v>88376.681500000006</v>
+      </c>
+      <c r="E90" s="2">
+        <v>429294.74939999997</v>
       </c>
       <c r="F90" s="2">
         <v>0.30980000000000002</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -3603,17 +3009,17 @@
       <c r="C91" s="1">
         <v>3</v>
       </c>
-      <c r="D91" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>190</v>
+      <c r="D91" s="2">
+        <v>88375.705400000006</v>
+      </c>
+      <c r="E91" s="2">
+        <v>429295.82120000001</v>
       </c>
       <c r="F91" s="2">
         <v>-0.15959999999999999</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -3626,11 +3032,11 @@
       <c r="C92" s="1">
         <v>4</v>
       </c>
-      <c r="D92" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>192</v>
+      <c r="D92" s="2">
+        <v>88375.785499999998</v>
+      </c>
+      <c r="E92" s="2">
+        <v>429295.72659999999</v>
       </c>
       <c r="F92" s="2">
         <v>-0.40699999999999997</v>
@@ -3649,17 +3055,17 @@
       <c r="C93" s="1">
         <v>1</v>
       </c>
-      <c r="D93" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>194</v>
+      <c r="D93" s="2">
+        <v>88373.734700000001</v>
+      </c>
+      <c r="E93" s="2">
+        <v>429317.20799999998</v>
       </c>
       <c r="F93" s="2">
         <v>0.53520000000000001</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -3672,17 +3078,17 @@
       <c r="C94" s="1">
         <v>2</v>
       </c>
-      <c r="D94" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>196</v>
+      <c r="D94" s="2">
+        <v>88375.004100000006</v>
+      </c>
+      <c r="E94" s="2">
+        <v>429317.25199999998</v>
       </c>
       <c r="F94" s="2">
         <v>0.44629999999999997</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -3695,17 +3101,17 @@
       <c r="C95" s="1">
         <v>3</v>
       </c>
-      <c r="D95" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>198</v>
+      <c r="D95" s="2">
+        <v>88376.409299999999</v>
+      </c>
+      <c r="E95" s="2">
+        <v>429317.25290000002</v>
       </c>
       <c r="F95" s="2">
         <v>-0.26079999999999998</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -3718,11 +3124,11 @@
       <c r="C96" s="1">
         <v>4</v>
       </c>
-      <c r="D96" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>200</v>
+      <c r="D96" s="2">
+        <v>88376.530199999994</v>
+      </c>
+      <c r="E96" s="2">
+        <v>429317.25280000002</v>
       </c>
       <c r="F96" s="2">
         <v>-0.36890000000000001</v>
@@ -3741,17 +3147,17 @@
       <c r="C97" s="1">
         <v>1</v>
       </c>
-      <c r="D97" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>202</v>
+      <c r="D97" s="2">
+        <v>88387.788799999995</v>
+      </c>
+      <c r="E97" s="2">
+        <v>429318.17229999998</v>
       </c>
       <c r="F97" s="2">
         <v>6.8099999999999994E-2</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>209</v>
+        <v>11</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -3764,17 +3170,17 @@
       <c r="C98" s="1">
         <v>2</v>
       </c>
-      <c r="D98" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>204</v>
+      <c r="D98" s="2">
+        <v>88387.140799999994</v>
+      </c>
+      <c r="E98" s="2">
+        <v>429318.09600000002</v>
       </c>
       <c r="F98" s="2">
         <v>-0.28910000000000002</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -3787,17 +3193,17 @@
       <c r="C99" s="1">
         <v>3</v>
       </c>
-      <c r="D99" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>206</v>
+      <c r="D99" s="2">
+        <v>88385.560700000002</v>
+      </c>
+      <c r="E99" s="2">
+        <v>429318.16850000003</v>
       </c>
       <c r="F99" s="2">
         <v>-0.34300000000000003</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -3810,11 +3216,11 @@
       <c r="C100" s="1">
         <v>4</v>
       </c>
-      <c r="D100" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>208</v>
+      <c r="D100" s="2">
+        <v>88385.230899999995</v>
+      </c>
+      <c r="E100" s="2">
+        <v>429318.17320000002</v>
       </c>
       <c r="F100" s="2">
         <v>-0.34670000000000001</v>
@@ -3824,7 +3230,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G100"/>
+  <autoFilter ref="A1:G100" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>